<commit_message>
restructure as scripting dictionary
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\stimuli with coding macros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11F4DBA-2D4E-41CD-80BB-A1C81B21C199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84272DC3-B09F-4D0F-873B-313E005A03AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2320" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
-  <si>
-    <t>video_id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>participant</t>
   </si>
   <si>
     <t>test_date</t>
@@ -48,6 +51,9 @@
     <t>gender</t>
   </si>
   <si>
+    <t>race</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -87,136 +93,106 @@
     <t>video</t>
   </si>
   <si>
-    <t>audio</t>
+    <t>sound</t>
   </si>
   <si>
     <t>fun</t>
   </si>
   <si>
-    <t>consent_level</t>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>fill manually from REDCap</t>
+  </si>
+  <si>
+    <t>condition2</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>pinkberries</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>a little easy</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>condition1</t>
+  </si>
+  <si>
+    <t>ipad</t>
+  </si>
+  <si>
+    <t>blueberries</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>very hard</t>
+  </si>
+  <si>
+    <t>bbbbbbbb</t>
+  </si>
+  <si>
+    <t>cccccccc</t>
+  </si>
+  <si>
+    <t>laptop 14"</t>
+  </si>
+  <si>
+    <t>studyname_20201214_01</t>
+  </si>
+  <si>
+    <t>studyname_20201215_03</t>
+  </si>
+  <si>
+    <t>condition3</t>
+  </si>
+  <si>
+    <t>dddddd</t>
+  </si>
+  <si>
+    <t>studyname_20201215_02</t>
   </si>
   <si>
     <t>studyname_20201215_01</t>
-  </si>
-  <si>
-    <t>MZ</t>
-  </si>
-  <si>
-    <t>Zoom</t>
-  </si>
-  <si>
-    <t>fill manually from REDCap</t>
-  </si>
-  <si>
-    <t>condition1</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>ipad</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>blueberries</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>hard</t>
-  </si>
-  <si>
-    <t>very hard</t>
-  </si>
-  <si>
-    <t>aaaaaaaaa</t>
-  </si>
-  <si>
-    <t>studyname_20201215_02</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>condition2</t>
-  </si>
-  <si>
-    <t>laptop 13"</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>pinkberries</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
-    <t>easy</t>
-  </si>
-  <si>
-    <t>a little easy</t>
-  </si>
-  <si>
-    <t>bbbbbbbbbbb</t>
-  </si>
-  <si>
-    <t>studyname_20201215_03</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>condition3</t>
-  </si>
-  <si>
-    <t>laptop 16"</t>
-  </si>
-  <si>
-    <t>a little hard</t>
-  </si>
-  <si>
-    <t>cccccccc</t>
-  </si>
-  <si>
-    <t>participant</t>
-  </si>
-  <si>
-    <t>asdasfd</t>
-  </si>
-  <si>
-    <t>studyname_20201214_01</t>
-  </si>
-  <si>
-    <t>studyname_20201215_04</t>
-  </si>
-  <si>
-    <t>very easy</t>
-  </si>
-  <si>
-    <t>asijerjw</t>
-  </si>
-  <si>
-    <t>studyname_20201215_05</t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>aselrklkjer</t>
   </si>
 </sst>
 </file>
@@ -535,96 +511,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="13" max="13" width="15.08984375" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" customWidth="1"/>
+    <col min="20" max="20" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -648,13 +634,13 @@
         <v>26</v>
       </c>
       <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -683,8 +669,8 @@
       <c r="T2" t="s">
         <v>37</v>
       </c>
-      <c r="U2">
-        <v>2</v>
+      <c r="U2" t="s">
+        <v>29</v>
       </c>
       <c r="V2">
         <v>3</v>
@@ -693,12 +679,15 @@
         <v>4</v>
       </c>
       <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -707,7 +696,7 @@
         <v>44180</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -722,57 +711,60 @@
         <v>26</v>
       </c>
       <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" t="s">
         <v>41</v>
       </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3">
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
         <v>5</v>
       </c>
-      <c r="V3">
+      <c r="Y3">
         <v>2</v>
       </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -781,7 +773,7 @@
         <v>44180</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -796,57 +788,60 @@
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
       <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
         <v>42</v>
-      </c>
-      <c r="M4" t="s">
-        <v>43</v>
       </c>
       <c r="N4" t="s">
         <v>32</v>
       </c>
       <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
-        <v>33</v>
-      </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
       </c>
       <c r="S4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="T4" t="s">
-        <v>54</v>
-      </c>
-      <c r="U4">
+        <v>48</v>
+      </c>
+      <c r="U4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
         <v>3</v>
       </c>
-      <c r="V4">
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="Y4">
         <v>2</v>
       </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>3</v>
-      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -870,22 +865,22 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="K5" t="s">
-        <v>29</v>
-      </c>
       <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
         <v>33</v>
@@ -903,166 +898,21 @@
         <v>36</v>
       </c>
       <c r="T5" t="s">
-        <v>56</v>
-      </c>
-      <c r="U5">
+        <v>53</v>
+      </c>
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5">
         <v>2</v>
       </c>
-      <c r="V5">
-        <v>3</v>
-      </c>
       <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
         <v>4</v>
       </c>
-      <c r="X5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44180</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6" t="s">
-        <v>59</v>
-      </c>
-      <c r="T6" t="s">
-        <v>60</v>
-      </c>
-      <c r="U6">
-        <v>5</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>2</v>
-      </c>
-      <c r="X6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44180</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" t="s">
-        <v>59</v>
-      </c>
-      <c r="T7" t="s">
-        <v>63</v>
-      </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
-      <c r="V7">
-        <v>5</v>
-      </c>
-      <c r="W7">
-        <v>4</v>
-      </c>
-      <c r="X7">
+      <c r="Y5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add userform screenshots, reorder consent to match appt tracking sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84272DC3-B09F-4D0F-873B-313E005A03AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBD2FFF-0051-431B-8F76-73C7BB8D8672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2320" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2750" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
   <si>
     <t>file</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>studyname_20201215_01</t>
+  </si>
+  <si>
+    <t>studyname_20201216_01</t>
+  </si>
+  <si>
+    <t>a little hard</t>
+  </si>
+  <si>
+    <t>eeeeeeeeee</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>jumped around slides in a random order!</t>
+  </si>
+  <si>
+    <t>studyname_20201216_02</t>
+  </si>
+  <si>
+    <t>studyname_20201217_01</t>
+  </si>
+  <si>
+    <t>blah</t>
   </si>
 </sst>
 </file>
@@ -511,19 +535,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" customWidth="1"/>
-    <col min="18" max="18" width="13.36328125" customWidth="1"/>
+    <col min="13" max="13" width="11.7265625" customWidth="1"/>
+    <col min="18" max="18" width="11.26953125" customWidth="1"/>
     <col min="19" max="19" width="13.1796875" customWidth="1"/>
     <col min="20" max="20" width="16.453125" customWidth="1"/>
   </cols>
@@ -590,19 +617,19 @@
         <v>20</v>
       </c>
       <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>38</v>
       </c>
       <c r="Z1" t="s">
         <v>39</v>
@@ -616,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>44180</v>
+        <v>44179</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -669,20 +696,20 @@
       <c r="T2" t="s">
         <v>37</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>3</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>4</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>5</v>
-      </c>
-      <c r="Y2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
@@ -746,20 +773,20 @@
       <c r="T3" t="s">
         <v>47</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
         <v>41</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>3</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>4</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>5</v>
-      </c>
-      <c r="Y3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
@@ -823,20 +850,20 @@
       <c r="T4" t="s">
         <v>48</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
         <v>49</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>3</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>5</v>
-      </c>
-      <c r="Y4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
@@ -900,20 +927,251 @@
       <c r="T5" t="s">
         <v>53</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5" t="s">
         <v>41</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>2</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>5</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>4</v>
       </c>
-      <c r="Y5">
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6">
         <v>2</v>
+      </c>
+      <c r="V6" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>3</v>
+      </c>
+      <c r="Y6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44182</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement resource allocation measure
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBD2FFF-0051-431B-8F76-73C7BB8D8672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B2C8ED-41A4-4E0A-A07F-0BB7AD4567EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2750" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
   <si>
     <t>file</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Zoom</t>
   </si>
   <si>
-    <t>fill manually from REDCap</t>
-  </si>
-  <si>
     <t>condition2</t>
   </si>
   <si>
@@ -217,6 +214,81 @@
   </si>
   <si>
     <t>blah</t>
+  </si>
+  <si>
+    <t>atypical_dev</t>
+  </si>
+  <si>
+    <t>insuff_lang</t>
+  </si>
+  <si>
+    <t>parental_interference</t>
+  </si>
+  <si>
+    <t>exp_error</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>studyname_20201217_02</t>
+  </si>
+  <si>
+    <t>measure9</t>
+  </si>
+  <si>
+    <t>measure10</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>in_progress</t>
+  </si>
+  <si>
+    <t>studyname_20201217_03</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>stopped and resumed in middle</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>very easy</t>
+  </si>
+  <si>
+    <t>testing resource allocation in progress</t>
+  </si>
+  <si>
+    <t>3_3</t>
+  </si>
+  <si>
+    <t>4_2</t>
+  </si>
+  <si>
+    <t>android phone</t>
+  </si>
+  <si>
+    <t>testing in progress functionality</t>
+  </si>
+  <si>
+    <t>5_1</t>
+  </si>
+  <si>
+    <t>6_0</t>
+  </si>
+  <si>
+    <t>studyname_20201217_04</t>
+  </si>
+  <si>
+    <t>allocation reset test</t>
+  </si>
+  <si>
+    <t>studyname_20201217_05</t>
   </si>
 </sst>
 </file>
@@ -535,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,15 +619,18 @@
     <col min="2" max="2" width="10.36328125" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" customWidth="1"/>
     <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="7" width="5.1796875" customWidth="1"/>
     <col min="9" max="9" width="14.453125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" customWidth="1"/>
-    <col min="19" max="19" width="13.1796875" customWidth="1"/>
-    <col min="20" max="20" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="11.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" customWidth="1"/>
+    <col min="26" max="26" width="16.453125" customWidth="1"/>
+    <col min="27" max="27" width="13.08984375" customWidth="1"/>
+    <col min="28" max="28" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,54 +665,78 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -651,70 +750,61 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2">
-        <v>2</v>
-      </c>
-      <c r="V2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2">
+      <c r="AE2">
         <v>3</v>
       </c>
-      <c r="X2">
+      <c r="AF2">
         <v>4</v>
       </c>
-      <c r="Y2">
+      <c r="AG2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -728,70 +818,61 @@
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
       <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" t="s">
-        <v>47</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3">
+      <c r="AE3">
         <v>3</v>
       </c>
-      <c r="X3">
+      <c r="AF3">
         <v>4</v>
       </c>
-      <c r="Y3">
+      <c r="AG3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -805,70 +886,61 @@
       <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="W4" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y4" t="s">
         <v>35</v>
       </c>
-      <c r="S4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="Z4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="s">
         <v>48</v>
       </c>
-      <c r="U4">
-        <v>2</v>
-      </c>
-      <c r="V4" t="s">
-        <v>49</v>
-      </c>
-      <c r="W4">
+      <c r="AE4">
         <v>1</v>
       </c>
-      <c r="X4">
+      <c r="AF4">
         <v>3</v>
       </c>
-      <c r="Y4">
+      <c r="AG4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -882,70 +954,61 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
       <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" t="s">
         <v>52</v>
       </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" t="s">
-        <v>53</v>
-      </c>
-      <c r="U5">
+      <c r="AC5">
         <v>2</v>
       </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5">
+      <c r="AD5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5">
         <v>2</v>
       </c>
-      <c r="X5">
+      <c r="AF5">
         <v>5</v>
       </c>
-      <c r="Y5">
+      <c r="AG5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -959,70 +1022,61 @@
       <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R6" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" t="s">
-        <v>57</v>
-      </c>
-      <c r="T6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U6">
+      <c r="AE6">
         <v>2</v>
       </c>
-      <c r="V6" t="s">
-        <v>29</v>
-      </c>
-      <c r="W6">
-        <v>2</v>
-      </c>
-      <c r="X6">
+      <c r="AF6">
         <v>3</v>
       </c>
-      <c r="Y6">
+      <c r="AG6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1036,70 +1090,61 @@
       <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="R7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" t="s">
         <v>35</v>
       </c>
-      <c r="S7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" t="s">
-        <v>60</v>
-      </c>
-      <c r="U7">
+      <c r="Z7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC7">
         <v>1</v>
       </c>
-      <c r="V7" t="s">
-        <v>59</v>
-      </c>
-      <c r="W7">
+      <c r="AD7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE7">
         <v>1</v>
       </c>
-      <c r="X7">
+      <c r="AF7">
         <v>4</v>
       </c>
-      <c r="Y7">
+      <c r="AG7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1113,65 +1158,346 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W8" t="s">
+        <v>43</v>
+      </c>
+      <c r="X8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+      <c r="AF8">
+        <v>3</v>
+      </c>
+      <c r="AG8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44182</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T9" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" t="s">
+        <v>32</v>
+      </c>
+      <c r="W9" t="s">
+        <v>33</v>
+      </c>
+      <c r="X9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE9">
+        <v>5</v>
+      </c>
+      <c r="AF9">
+        <v>4</v>
+      </c>
+      <c r="AG9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T10" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10" t="s">
+        <v>33</v>
+      </c>
+      <c r="X10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE10">
+        <v>3</v>
+      </c>
+      <c r="AF10">
+        <v>2</v>
+      </c>
+      <c r="AG10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44182</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" t="s">
+        <v>71</v>
+      </c>
+      <c r="R11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" t="s">
         <v>33</v>
       </c>
-      <c r="L8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="X11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE11">
+        <v>4</v>
+      </c>
+      <c r="AF11">
+        <v>2</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44182</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" t="s">
         <v>42</v>
       </c>
-      <c r="N8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="U12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V12" t="s">
+        <v>32</v>
+      </c>
+      <c r="W12" t="s">
         <v>33</v>
       </c>
-      <c r="P8" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="X12" t="s">
         <v>44</v>
       </c>
-      <c r="R8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" t="s">
-        <v>36</v>
-      </c>
-      <c r="T8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U8">
+      <c r="Y12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC12">
         <v>3</v>
       </c>
-      <c r="V8" t="s">
-        <v>29</v>
-      </c>
-      <c r="W8">
+      <c r="AD12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE12">
+        <v>3</v>
+      </c>
+      <c r="AF12">
         <v>2</v>
       </c>
-      <c r="X8">
-        <v>3</v>
-      </c>
-      <c r="Y8">
-        <v>4</v>
+      <c r="AG12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reimplement resource allocation and reset between anchor objects
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E200877-D56A-467A-8842-65D86A8FEDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA28523-F8DB-44E6-88D2-19CB2DCC9087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
   <si>
     <t>file</t>
   </si>
@@ -141,9 +141,6 @@
     <t>condition1</t>
   </si>
   <si>
-    <t>ipad</t>
-  </si>
-  <si>
     <t>blueberries</t>
   </si>
   <si>
@@ -156,33 +153,12 @@
     <t>very hard</t>
   </si>
   <si>
-    <t>bbbbbbbb</t>
-  </si>
-  <si>
-    <t>cccccccc</t>
-  </si>
-  <si>
-    <t>laptop 14"</t>
-  </si>
-  <si>
     <t>studyname_20201214_01</t>
   </si>
   <si>
-    <t>studyname_20201215_03</t>
-  </si>
-  <si>
     <t>condition3</t>
   </si>
   <si>
-    <t>dddddd</t>
-  </si>
-  <si>
-    <t>studyname_20201215_02</t>
-  </si>
-  <si>
-    <t>studyname_20201215_01</t>
-  </si>
-  <si>
     <t>studyname_20201216_01</t>
   </si>
   <si>
@@ -204,9 +180,6 @@
     <t>studyname_20201217_01</t>
   </si>
   <si>
-    <t>blah</t>
-  </si>
-  <si>
     <t>atypical_dev</t>
   </si>
   <si>
@@ -225,12 +198,6 @@
     <t>studyname_20201217_02</t>
   </si>
   <si>
-    <t>measure9</t>
-  </si>
-  <si>
-    <t>measure10</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -252,36 +219,15 @@
     <t>very easy</t>
   </si>
   <si>
-    <t>testing resource allocation in progress</t>
-  </si>
-  <si>
-    <t>3_3</t>
-  </si>
-  <si>
-    <t>4_2</t>
-  </si>
-  <si>
     <t>android phone</t>
   </si>
   <si>
     <t>testing in progress functionality</t>
   </si>
   <si>
-    <t>5_1</t>
-  </si>
-  <si>
-    <t>6_0</t>
-  </si>
-  <si>
-    <t>studyname_20201217_04</t>
-  </si>
-  <si>
     <t>allocation reset test</t>
   </si>
   <si>
-    <t>studyname_20201217_05</t>
-  </si>
-  <si>
     <t>measure6_button1</t>
   </si>
   <si>
@@ -307,6 +253,33 @@
   </si>
   <si>
     <t>testing measure 6 buttons</t>
+  </si>
+  <si>
+    <t>studyname_20201218_02</t>
+  </si>
+  <si>
+    <t>measure10_highPerf_anchor</t>
+  </si>
+  <si>
+    <t>measure10_lowPerf_anchor</t>
+  </si>
+  <si>
+    <t>measure9_highPerf_anchor</t>
+  </si>
+  <si>
+    <t>measure9_lowPerf_anchor</t>
+  </si>
+  <si>
+    <t>studyname_20201218_03</t>
+  </si>
+  <si>
+    <t>testing allocation</t>
+  </si>
+  <si>
+    <t>chromebook</t>
+  </si>
+  <si>
+    <t>testing allocation reset</t>
   </si>
 </sst>
 </file>
@@ -632,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM13"/>
+  <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,11 +627,13 @@
     <col min="29" max="29" width="11.26953125" customWidth="1"/>
     <col min="30" max="30" width="13.1796875" customWidth="1"/>
     <col min="31" max="31" width="16.453125" customWidth="1"/>
-    <col min="32" max="32" width="13.08984375" customWidth="1"/>
-    <col min="33" max="33" width="13.90625" customWidth="1"/>
+    <col min="32" max="32" width="24.81640625" customWidth="1"/>
+    <col min="33" max="33" width="24.90625" customWidth="1"/>
+    <col min="34" max="34" width="25.90625" customWidth="1"/>
+    <col min="35" max="35" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,22 +668,22 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>12</v>
@@ -726,22 +701,22 @@
         <v>16</v>
       </c>
       <c r="W1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="X1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="Y1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="Z1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="AA1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="AB1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="AC1" t="s">
         <v>17</v>
@@ -753,33 +728,39 @@
         <v>19</v>
       </c>
       <c r="AF1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="AG1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AH1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>11</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>22</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -800,7 +781,7 @@
         <v>26</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>28</v>
@@ -826,31 +807,31 @@
       <c r="AE2" t="s">
         <v>34</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2">
         <v>2</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2">
+      <c r="AL2">
         <v>3</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>4</v>
       </c>
-      <c r="AL2">
+      <c r="AN2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>44180</v>
+        <v>44181</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -859,63 +840,63 @@
         <v>24</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" t="s">
         <v>40</v>
       </c>
-      <c r="U3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>41</v>
-      </c>
       <c r="AD3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AE3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH3">
+        <v>46</v>
+      </c>
+      <c r="AJ3">
         <v>2</v>
       </c>
-      <c r="AI3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3">
+      <c r="AK3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL3">
+        <v>2</v>
+      </c>
+      <c r="AM3">
         <v>3</v>
       </c>
-      <c r="AK3">
-        <v>4</v>
-      </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>44180</v>
+        <v>44181</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -924,19 +905,19 @@
         <v>24</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>30</v>
@@ -954,33 +935,33 @@
         <v>33</v>
       </c>
       <c r="AE4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH4">
-        <v>2</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AJ4">
         <v>1</v>
       </c>
-      <c r="AK4">
-        <v>3</v>
+      <c r="AK4" t="s">
+        <v>47</v>
       </c>
       <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>4</v>
+      </c>
+      <c r="AN4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>44180</v>
+        <v>44182</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -989,63 +970,63 @@
         <v>24</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" t="s">
         <v>40</v>
       </c>
-      <c r="U5" t="s">
-        <v>31</v>
-      </c>
-      <c r="V5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>32</v>
-      </c>
       <c r="AD5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="AE5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH5">
-        <v>2</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="AJ5">
-        <v>2</v>
-      </c>
-      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL5">
         <v>5</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>4</v>
       </c>
+      <c r="AN5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>44181</v>
+        <v>44182</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -1054,63 +1035,63 @@
         <v>24</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="U6" t="s">
         <v>31</v>
       </c>
       <c r="V6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="AC6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="AD6" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="AE6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH6">
+        <v>65</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL6">
+        <v>4</v>
+      </c>
+      <c r="AM6">
         <v>2</v>
       </c>
-      <c r="AI6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ6">
-        <v>2</v>
-      </c>
-      <c r="AK6">
-        <v>3</v>
-      </c>
-      <c r="AL6">
-        <v>5</v>
+      <c r="AN6">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>44181</v>
+        <v>44182</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -1125,57 +1106,57 @@
         <v>31</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="U7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="V7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="AC7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AD7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AE7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH7">
-        <v>1</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="AJ7">
-        <v>1</v>
-      </c>
-      <c r="AK7">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>62</v>
       </c>
       <c r="AL7">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="AM7">
+        <v>2</v>
+      </c>
+      <c r="AN7">
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -1184,63 +1165,72 @@
         <v>24</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="U8" t="s">
         <v>31</v>
       </c>
       <c r="V8" t="s">
         <v>31</v>
       </c>
+      <c r="W8" t="s">
+        <v>74</v>
+      </c>
+      <c r="X8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>74</v>
+      </c>
       <c r="AC8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AD8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AE8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH8">
-        <v>3</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="AJ8">
-        <v>2</v>
-      </c>
-      <c r="AK8">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>47</v>
       </c>
       <c r="AL8">
         <v>4</v>
       </c>
+      <c r="AM8">
+        <v>2</v>
+      </c>
+      <c r="AN8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -1249,19 +1239,19 @@
         <v>24</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="T9" s="2" t="s">
         <v>30</v>
@@ -1270,42 +1260,66 @@
         <v>26</v>
       </c>
       <c r="V9" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="X9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>74</v>
       </c>
       <c r="AC9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="AD9" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="AE9" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>6</v>
       </c>
       <c r="AH9">
-        <v>1</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>71</v>
+        <v>4</v>
+      </c>
+      <c r="AI9">
+        <v>2</v>
       </c>
       <c r="AJ9">
-        <v>5</v>
-      </c>
-      <c r="AK9">
+        <v>3</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL9">
         <v>4</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
+        <v>2</v>
+      </c>
+      <c r="AN9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -1314,19 +1328,19 @@
         <v>24</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>30</v>
@@ -1337,257 +1351,50 @@
       <c r="V10" t="s">
         <v>26</v>
       </c>
+      <c r="X10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>74</v>
+      </c>
       <c r="AC10" t="s">
         <v>32</v>
       </c>
       <c r="AD10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="AE10" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>77</v>
+        <v>84</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>6</v>
       </c>
       <c r="AH10">
+        <v>4</v>
+      </c>
+      <c r="AI10">
         <v>2</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>73</v>
       </c>
       <c r="AJ10">
         <v>3</v>
       </c>
-      <c r="AK10">
-        <v>2</v>
+      <c r="AK10" t="s">
+        <v>83</v>
       </c>
       <c r="AL10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44182</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH11">
-        <v>1</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ11">
-        <v>4</v>
-      </c>
-      <c r="AK11">
+      <c r="AM10">
         <v>2</v>
       </c>
-      <c r="AL11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44182</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" t="s">
-        <v>26</v>
-      </c>
-      <c r="V12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH12">
+      <c r="AN10">
         <v>3</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ12">
-        <v>3</v>
-      </c>
-      <c r="AK12">
-        <v>2</v>
-      </c>
-      <c r="AL12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44183</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U13" t="s">
-        <v>31</v>
-      </c>
-      <c r="V13" t="s">
-        <v>31</v>
-      </c>
-      <c r="W13" t="s">
-        <v>92</v>
-      </c>
-      <c r="X13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH13">
-        <v>1</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ13">
-        <v>4</v>
-      </c>
-      <c r="AK13">
-        <v>2</v>
-      </c>
-      <c r="AL13">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make setup save to excel to keep participants blind to condition
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA28523-F8DB-44E6-88D2-19CB2DCC9087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECF7CE5-8DC7-4231-BCFC-11A5F7FD0D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2750" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="87">
   <si>
     <t>file</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>testing allocation reset</t>
+  </si>
+  <si>
+    <t>studyname_20201218_04</t>
+  </si>
+  <si>
+    <t>test quit, resume after setup</t>
   </si>
 </sst>
 </file>
@@ -605,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO10"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="AH13" sqref="AH13"/>
@@ -1397,6 +1403,95 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF11">
+        <v>2</v>
+      </c>
+      <c r="AG11">
+        <v>4</v>
+      </c>
+      <c r="AH11">
+        <v>3</v>
+      </c>
+      <c r="AI11">
+        <v>3</v>
+      </c>
+      <c r="AJ11">
+        <v>3</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL11">
+        <v>4</v>
+      </c>
+      <c r="AM11">
+        <v>2</v>
+      </c>
+      <c r="AN11">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clean anchor names before storing as allocation keys
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECF7CE5-8DC7-4231-BCFC-11A5F7FD0D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B5DD77-2887-41EA-94C5-1F09C07B9042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2750" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="90">
   <si>
     <t>file</t>
   </si>
@@ -258,18 +258,6 @@
     <t>studyname_20201218_02</t>
   </si>
   <si>
-    <t>measure10_highPerf_anchor</t>
-  </si>
-  <si>
-    <t>measure10_lowPerf_anchor</t>
-  </si>
-  <si>
-    <t>measure9_highPerf_anchor</t>
-  </si>
-  <si>
-    <t>measure9_lowPerf_anchor</t>
-  </si>
-  <si>
     <t>studyname_20201218_03</t>
   </si>
   <si>
@@ -286,6 +274,27 @@
   </si>
   <si>
     <t>test quit, resume after setup</t>
+  </si>
+  <si>
+    <t>measure9_lowPerf</t>
+  </si>
+  <si>
+    <t>measure9_highPerf</t>
+  </si>
+  <si>
+    <t>measure10_highPerf</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>testing allocation anchor name cleaning</t>
+  </si>
+  <si>
+    <t>measure10_lowPerf</t>
+  </si>
+  <si>
+    <t>studyname_20201218_05</t>
   </si>
 </sst>
 </file>
@@ -611,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO11"/>
+  <dimension ref="A1:AO12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,9 +642,9 @@
     <col min="29" max="29" width="11.26953125" customWidth="1"/>
     <col min="30" max="30" width="13.1796875" customWidth="1"/>
     <col min="31" max="31" width="16.453125" customWidth="1"/>
-    <col min="32" max="32" width="24.81640625" customWidth="1"/>
-    <col min="33" max="33" width="24.90625" customWidth="1"/>
-    <col min="34" max="34" width="25.90625" customWidth="1"/>
+    <col min="32" max="32" width="27.1796875" customWidth="1"/>
+    <col min="33" max="33" width="24.81640625" customWidth="1"/>
+    <col min="34" max="34" width="24.90625" customWidth="1"/>
     <col min="35" max="35" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -734,16 +743,16 @@
         <v>19</v>
       </c>
       <c r="AF1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AG1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AH1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AJ1" t="s">
         <v>35</v>
@@ -1287,7 +1296,7 @@
         <v>63</v>
       </c>
       <c r="AE9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -1319,7 +1328,7 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1373,7 +1382,7 @@
         <v>63</v>
       </c>
       <c r="AE10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AF10">
         <v>0</v>
@@ -1391,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="AK10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AL10">
         <v>3</v>
@@ -1405,7 +1414,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1462,7 +1471,7 @@
         <v>63</v>
       </c>
       <c r="AE11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AF11">
         <v>2</v>
@@ -1480,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="AK11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AL11">
         <v>4</v>
@@ -1490,6 +1499,92 @@
       </c>
       <c r="AN11">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44183</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U12" t="s">
+        <v>31</v>
+      </c>
+      <c r="V12" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>5</v>
+      </c>
+      <c r="AH12">
+        <v>4</v>
+      </c>
+      <c r="AI12">
+        <v>2</v>
+      </c>
+      <c r="AJ12">
+        <v>3</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL12">
+        <v>3</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AN12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>